<commit_message>
Refactorización completa y funcional
El bot se encuentra funcionando completamente.
</commit_message>
<xml_diff>
--- a/Qualis-Bot-SalesNavigator/KeyboardInputEmpresa.xlsx
+++ b/Qualis-Bot-SalesNavigator/KeyboardInputEmpresa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Cruz Diana\Documents\GitHub\SalesBot\Qualis-Bot-SalesNavigator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E0889-BC6A-4DB2-8C19-6FBC9D7BE354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67404E58-C6E0-426B-AE8B-2D228091B0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCandidatos" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
   <si>
     <t>CIO</t>
   </si>
@@ -370,13 +370,16 @@
   </si>
   <si>
     <t>QA</t>
+  </si>
+  <si>
+    <t>Representante visitador médico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +400,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -492,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,6 +521,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,7 +920,7 @@
   <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,8 +1520,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="5"/>
+    <row r="119" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A119" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="120" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>

</xml_diff>